<commit_message>
Add Expected Result to importer and related tests.
</commit_message>
<xml_diff>
--- a/VM-Core/src/test/java/com/validation/manager/core/tool/step/importer/Reqs.xlsx
+++ b/VM-Core/src/test/java/com/validation/manager/core/tool/step/importer/Reqs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="27">
   <si>
     <t>Description 1</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>SRS-SW-0001</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -433,9 +439,10 @@
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -446,10 +453,13 @@
         <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -459,19 +469,22 @@
       <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -481,19 +494,22 @@
       <c r="C4" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -503,19 +519,22 @@
       <c r="C6" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -525,19 +544,22 @@
       <c r="C8" t="s">
         <v>24</v>
       </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -547,19 +569,22 @@
       <c r="C10" t="s">
         <v>24</v>
       </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -569,19 +594,22 @@
       <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="D13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>13</v>
       </c>
@@ -591,19 +619,22 @@
       <c r="C14" t="s">
         <v>24</v>
       </c>
-      <c r="D14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="D15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>15</v>
       </c>
@@ -613,19 +644,22 @@
       <c r="C16" t="s">
         <v>24</v>
       </c>
-      <c r="D16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18">
         <v>17</v>
       </c>
@@ -635,19 +669,22 @@
       <c r="C18" t="s">
         <v>24</v>
       </c>
-      <c r="D18" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20">
         <v>19</v>
       </c>
@@ -657,16 +694,19 @@
       <c r="C20" t="s">
         <v>24</v>
       </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
+      </c>
+      <c r="D21" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>